<commit_message>
Added some text properties to ensure they're ignored
</commit_message>
<xml_diff>
--- a/tests/fixtures/ooffice_exotic_sheet.xlsx
+++ b/tests/fixtures/ooffice_exotic_sheet.xlsx
@@ -59,7 +59,7 @@
     <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="167" formatCode="D&quot;. &quot;MMM&quot;. &quot;YYYY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -90,7 +90,15 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="DejaVu Sans"/>
+      <color rgb="FFCE181E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -136,7 +144,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -157,7 +165,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -174,6 +186,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -185,10 +257,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.29"/>
@@ -236,7 +308,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="n">
@@ -263,8 +335,8 @@
       <c r="E4" s="3"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
@@ -279,7 +351,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="7" t="n">
         <v>54969</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deal with the very first column being NULL
</commit_message>
<xml_diff>
--- a/tests/fixtures/ooffice_exotic_sheet.xlsx
+++ b/tests/fixtures/ooffice_exotic_sheet.xlsx
@@ -98,7 +98,7 @@
     <font>
       <u val="single"/>
       <sz val="10"/>
-      <name val="Noto Sans CJK SC Regular"/>
+      <name val="DejaVu Sans"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -254,13 +254,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.29"/>
@@ -352,6 +352,22 @@
         <v>0</v>
       </c>
       <c r="F5" s="7" t="n">
+        <v>54969</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="2" t="n">
+        <v>-100</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <f aca="false">50+100-50</f>
+        <v>100</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="n">
         <v>54969</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Handle dates prior to the Excel epochs
</commit_message>
<xml_diff>
--- a/tests/fixtures/ooffice_exotic_sheet.xlsx
+++ b/tests/fixtures/ooffice_exotic_sheet.xlsx
@@ -254,10 +254,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -355,22 +355,6 @@
         <v>54969</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2" t="n">
-        <v>-100</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <f aca="false">50+100-50</f>
-        <v>100</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="7" t="n">
-        <v>54969</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>